<commit_message>
Ajout d'un fichier Excel pour gerer les balles
</commit_message>
<xml_diff>
--- a/VideoBalles/assets/ListeBalles.xlsx
+++ b/VideoBalles/assets/ListeBalles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\Documents\GitHub\tiktok_manager\VideoBalles\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7C5088-DB46-43B4-90DA-6CC21BCE7E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7888DBBB-EDC1-4AB6-A782-F75FDCDC8107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{02B7CA46-18BC-42BD-A073-B0E7CB583EC0}"/>
   </bookViews>
@@ -36,23 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Couleur Balle</t>
   </si>
   <si>
-    <t>Rayon balle</t>
-  </si>
-  <si>
     <t>Couleur Interieur Balle</t>
   </si>
   <si>
     <t>Taille Contour</t>
   </si>
   <si>
-    <t>Taille Trainée</t>
-  </si>
-  <si>
     <t>Texte</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>Couleur Rectangle Score</t>
   </si>
   <si>
-    <t>Couleur Texte score</t>
-  </si>
-  <si>
     <t>Acceleration</t>
   </si>
   <si>
@@ -135,6 +126,15 @@
   </si>
   <si>
     <t>1.jpg</t>
+  </si>
+  <si>
+    <t>Rayon Balle</t>
+  </si>
+  <si>
+    <t>Taille Trainee</t>
+  </si>
+  <si>
+    <t>Couleur Texte Score</t>
   </si>
 </sst>
 </file>
@@ -185,9 +185,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -200,19 +212,14 @@
       </extLst>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <extLst>
@@ -257,24 +264,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{047D9689-BF05-4502-AE97-80EADE8AADA6}" name="Tableau1" displayName="Tableau1" ref="A1:O7">
-  <autoFilter ref="A1:O7" xr:uid="{047D9689-BF05-4502-AE97-80EADE8AADA6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{047D9689-BF05-4502-AE97-80EADE8AADA6}" name="Tableau1" displayName="Tableau1" ref="A1:O6">
+  <autoFilter ref="A1:O6" xr:uid="{047D9689-BF05-4502-AE97-80EADE8AADA6}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{CB34F05D-A392-40F1-B343-180381EBFF50}" name="Afficher" totalsRowLabel="Total" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{CB34F05D-A392-40F1-B343-180381EBFF50}" name="Afficher" totalsRowLabel="Total" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{08BE89D9-A157-4F06-A086-DFCD4C59CA11}" name="INFOS"/>
-    <tableColumn id="8" xr3:uid="{3B37B40C-DBEB-40E3-9590-405F2A991B75}" name="Texte" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{43EE387F-F7F8-44A4-B416-1C991C1828E8}" name="Afficher Texte" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{3B37B40C-DBEB-40E3-9590-405F2A991B75}" name="Texte" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{43EE387F-F7F8-44A4-B416-1C991C1828E8}" name="Afficher Texte" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{A3B76A76-22BB-4FCE-BB24-904D08B07977}" name="Couleur Texte" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{4350E952-AA26-4181-A722-64FC122F2526}" name="Couleur Balle"/>
-    <tableColumn id="16" xr3:uid="{FBDE0901-02DC-4D23-A925-033B115CD615}" name="Image" dataDxfId="0"/>
+    <tableColumn id="16" xr3:uid="{FBDE0901-02DC-4D23-A925-033B115CD615}" name="Image" dataDxfId="5"/>
     <tableColumn id="13" xr3:uid="{FC727AA8-9DB1-4BCB-878B-78ACCB013E96}" name="Couleur Rectangle Score"/>
-    <tableColumn id="14" xr3:uid="{631E6625-8583-4F25-B9D4-E2EE6798BD97}" name="Couleur Texte score"/>
-    <tableColumn id="4" xr3:uid="{9D1C2EFC-0365-4D39-BEAD-4048F782AF5B}" name="Rayon balle" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{631E6625-8583-4F25-B9D4-E2EE6798BD97}" name="Couleur Texte Score"/>
+    <tableColumn id="4" xr3:uid="{9D1C2EFC-0365-4D39-BEAD-4048F782AF5B}" name="Rayon Balle" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{4F86DC08-4D23-48D4-B800-C3477A97072A}" name="Couleur Interieur Balle"/>
-    <tableColumn id="6" xr3:uid="{25B0C4FB-CC57-4788-8F79-CF3EBC60752A}" name="Taille Contour" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{1D6B7618-33F8-4CAA-A676-E20C7BB8498B}" name="Taille Trainée" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{D2C41EE0-C6A1-43A0-9560-8145C608F8DB}" name="Taille Font" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{A3B76A76-22BB-4FCE-BB24-904D08B07977}" name="Couleur Texte"/>
-    <tableColumn id="15" xr3:uid="{F1E8B700-9EA4-4EE5-BE2B-BF6D2C248379}" name="Acceleration" totalsRowFunction="sum" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{25B0C4FB-CC57-4788-8F79-CF3EBC60752A}" name="Taille Contour" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{1D6B7618-33F8-4CAA-A676-E20C7BB8498B}" name="Taille Trainee" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{D2C41EE0-C6A1-43A0-9560-8145C608F8DB}" name="Taille Font" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{F1E8B700-9EA4-4EE5-BE2B-BF6D2C248379}" name="Acceleration" totalsRowFunction="sum" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -597,317 +604,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5B4434-761B-4D40-92E9-037B049A5ECC}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="10.6640625" style="3"/>
     <col min="4" max="4" width="15.46484375" customWidth="1"/>
-    <col min="5" max="5" width="15.3984375" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="23.265625" customWidth="1"/>
-    <col min="8" max="8" width="18.86328125" customWidth="1"/>
-    <col min="9" max="9" width="11.86328125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" customWidth="1"/>
-    <col min="11" max="11" width="6.265625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="7.86328125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" style="2"/>
-    <col min="15" max="15" width="10.6640625" style="2"/>
-    <col min="17" max="17" width="22.33203125" customWidth="1"/>
-    <col min="18" max="18" width="20.06640625" customWidth="1"/>
-    <col min="19" max="19" width="12.73046875" customWidth="1"/>
+    <col min="5" max="5" width="12.265625" customWidth="1"/>
+    <col min="6" max="6" width="15.3984375" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="23.265625" customWidth="1"/>
+    <col min="9" max="9" width="18.86328125" customWidth="1"/>
+    <col min="10" max="10" width="11.86328125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" customWidth="1"/>
+    <col min="12" max="12" width="6.265625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="7.86328125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" style="2"/>
+    <col min="16" max="16" width="10.6640625" style="2"/>
+    <col min="18" max="18" width="22.33203125" customWidth="1"/>
+    <col min="19" max="19" width="20.06640625" customWidth="1"/>
+    <col min="20" max="20" width="12.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="P1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="2">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="2">
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="2">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="2">
         <v>2</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>10</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>25</v>
-      </c>
-      <c r="N2" t="s">
-        <v>18</v>
       </c>
       <c r="O2" s="2">
         <v>0.3</v>
       </c>
+      <c r="P2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="2">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2">
         <v>20</v>
       </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="2">
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="2">
         <v>2</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>10</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>25</v>
-      </c>
-      <c r="N3" t="s">
-        <v>18</v>
       </c>
       <c r="O3" s="2">
         <v>0.3</v>
       </c>
+      <c r="P3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="2">
-        <v>20</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="2">
-        <v>2</v>
-      </c>
-      <c r="L4" s="2">
-        <v>10</v>
-      </c>
-      <c r="M4" s="2">
-        <v>25</v>
-      </c>
-      <c r="N4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0.3</v>
-      </c>
+      <c r="O4" s="2"/>
+      <c r="P4"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="2">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="2">
         <v>20</v>
       </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="2">
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="2">
         <v>2</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>10</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>25</v>
-      </c>
-      <c r="N5" t="s">
-        <v>18</v>
       </c>
       <c r="O5" s="2">
         <v>0.3</v>
       </c>
+      <c r="P5"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="2">
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="2">
         <v>20</v>
       </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="2">
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="2">
         <v>2</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <v>10</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N6" s="2">
         <v>25</v>
-      </c>
-      <c r="N6" t="s">
-        <v>18</v>
       </c>
       <c r="O6" s="2">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>20</v>
-      </c>
-      <c r="J7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="2">
-        <v>2</v>
-      </c>
-      <c r="L7" s="2">
-        <v>10</v>
-      </c>
-      <c r="M7" s="2">
-        <v>25</v>
-      </c>
-      <c r="N7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O7" s="2">
-        <v>0.3</v>
-      </c>
+      <c r="P6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>